<commit_message>
[ANV] updated germanium spreadsheet
</commit_message>
<xml_diff>
--- a/levelfiles/spreadsheet/germanium.xlsx
+++ b/levelfiles/spreadsheet/germanium.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/villaa/Computing/nrCascadeSim/levelfiles/spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54430711-61DD-3942-94CF-17E301D06288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD263D5D-F8E8-7A48-95A7-9A29BDB66B66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="760" windowWidth="28040" windowHeight="17040" activeTab="2" xr2:uid="{2D1C8EBD-58BF-0748-ACC6-F1ED1991D975}"/>
+    <workbookView xWindow="380" yWindow="760" windowWidth="28040" windowHeight="17040" xr2:uid="{2D1C8EBD-58BF-0748-ACC6-F1ED1991D975}"/>
   </bookViews>
   <sheets>
     <sheet name="isotopes" sheetId="1" r:id="rId1"/>
     <sheet name="74-primary gammas" sheetId="2" r:id="rId2"/>
     <sheet name="71-primary gammas" sheetId="4" r:id="rId3"/>
+    <sheet name="73-primary gammas" sheetId="6" r:id="rId4"/>
+    <sheet name="75-primary gammas" sheetId="8" r:id="rId5"/>
+    <sheet name="77-primary gammas" sheetId="10" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="germanium74" localSheetId="1">'74-primary gammas'!$C$3:$C$261</definedName>
@@ -53,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="15">
   <si>
     <t>iso</t>
   </si>
@@ -160,13 +163,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -487,7 +492,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{269F673A-9A68-9948-B26F-F24DE369A567}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -675,8 +680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B338AC58-B202-DF40-A9D1-45CAD65F15D2}">
   <dimension ref="A1:G262"/>
   <sheetViews>
-    <sheetView topLeftCell="A233" workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3096,8 +3101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{776D4DF7-4947-4942-AC8B-DD4EC3016BF9}">
   <dimension ref="A1:G219"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D220" sqref="D220"/>
+    <sheetView topLeftCell="A213" workbookViewId="0">
+      <selection activeCell="B91" sqref="B91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3137,12 +3142,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
+    <row r="3" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
         <f>$E$1-C3</f>
         <v>7415.94</v>
       </c>
-      <c r="C3" s="1">
+      <c r="B3" s="3">
+        <v>1.6E-2</v>
+      </c>
+      <c r="C3" s="2">
         <v>0</v>
       </c>
     </row>
@@ -3164,12 +3172,15 @@
         <v>198.35400000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
+    <row r="6" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
         <f t="shared" si="0"/>
         <v>6916.0239999999994</v>
       </c>
-      <c r="C6" s="1">
+      <c r="B6" s="3">
+        <v>3.1E-2</v>
+      </c>
+      <c r="C6" s="2">
         <v>499.916</v>
       </c>
     </row>
@@ -3191,12 +3202,15 @@
         <v>589.74900000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
+    <row r="9" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
         <f t="shared" si="0"/>
         <v>6707.7509999999993</v>
       </c>
-      <c r="C9" s="1">
+      <c r="B9" s="3">
+        <v>3.8800000000000001E-2</v>
+      </c>
+      <c r="C9" s="2">
         <v>708.18899999999996</v>
       </c>
     </row>
@@ -3254,15 +3268,12 @@
         <v>886.94</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
+    <row r="16" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="6">
         <f t="shared" si="0"/>
         <v>6389.3709999999992</v>
       </c>
-      <c r="B16" s="3">
-        <v>2.9899999999999999E-2</v>
-      </c>
-      <c r="C16" s="2">
+      <c r="C16" s="6">
         <v>1026.569</v>
       </c>
     </row>
@@ -3275,12 +3286,15 @@
         <v>1037.8399999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
+    <row r="18" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
         <f t="shared" si="0"/>
         <v>6320.4249999999993</v>
       </c>
-      <c r="C18" s="1">
+      <c r="B18" s="3">
+        <v>1.5299999999999999E-2</v>
+      </c>
+      <c r="C18" s="2">
         <v>1095.5150000000001</v>
       </c>
     </row>
@@ -3293,12 +3307,15 @@
         <v>1096.1400000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="1">
+    <row r="20" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
         <f t="shared" si="0"/>
         <v>6276.5109999999995</v>
       </c>
-      <c r="C20" s="1">
+      <c r="B20" s="3">
+        <v>2.1399999999999999E-2</v>
+      </c>
+      <c r="C20" s="2">
         <v>1139.4290000000001</v>
       </c>
     </row>
@@ -3374,12 +3391,15 @@
         <v>1288.5899999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="1">
+    <row r="29" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="2">
         <f t="shared" si="0"/>
         <v>6117.2060000000001</v>
       </c>
-      <c r="C29" s="1">
+      <c r="B29" s="3">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="C29" s="2">
         <v>1298.7339999999999</v>
       </c>
     </row>
@@ -3401,12 +3421,15 @@
         <v>1378.6</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="1">
+    <row r="32" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="2">
         <f t="shared" si="0"/>
         <v>6037.2599999999993</v>
       </c>
-      <c r="C32" s="1">
+      <c r="B32" s="3">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="C32" s="2">
         <v>1378.68</v>
       </c>
     </row>
@@ -3518,12 +3541,15 @@
         <v>1566.1</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="1">
+    <row r="45" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="2">
         <f t="shared" si="0"/>
         <v>5817.4119999999994</v>
       </c>
-      <c r="C45" s="1">
+      <c r="B45" s="3">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="C45" s="2">
         <v>1598.528</v>
       </c>
     </row>
@@ -3689,12 +3715,15 @@
         <v>1959.67</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A64" s="1">
+    <row r="64" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="2">
         <f t="shared" si="0"/>
         <v>5450.91</v>
       </c>
-      <c r="C64" s="1">
+      <c r="B64" s="3">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="C64" s="2">
         <v>1965.03</v>
       </c>
     </row>
@@ -3707,12 +3736,15 @@
         <v>1979</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A66" s="1">
+    <row r="66" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="2">
         <f t="shared" si="0"/>
         <v>5383.9599999999991</v>
       </c>
-      <c r="C66" s="1">
+      <c r="B66" s="3">
+        <v>1.3100000000000001E-2</v>
+      </c>
+      <c r="C66" s="2">
         <v>2031.98</v>
       </c>
     </row>
@@ -3995,12 +4027,15 @@
         <v>2523</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A98" s="1">
+    <row r="98" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A98" s="2">
         <f t="shared" si="1"/>
         <v>4881.99</v>
       </c>
-      <c r="C98" s="1">
+      <c r="B98" s="3">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="C98" s="2">
         <v>2533.9499999999998</v>
       </c>
     </row>
@@ -5090,13 +5125,3370 @@
       </c>
       <c r="B219" s="4">
         <f>SUM(B3:B218)</f>
-        <v>2.9899999999999999E-2</v>
+        <v>0.29659999999999997</v>
       </c>
       <c r="C219" s="5">
         <f>(B219/G1)*100</f>
-        <v>1.3</v>
+        <v>12.895652173913044</v>
       </c>
       <c r="D219" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26A53988-4640-5749-8A6B-6016B85B6590}">
+  <dimension ref="A1:G146"/>
+  <sheetViews>
+    <sheetView topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="A146" sqref="A146:XFD146"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="21.5" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1">
+        <f>isotopes!F4*1000</f>
+        <v>6782.94</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <f>$E$1-C3</f>
+        <v>6782.94</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <f t="shared" ref="A4:A67" si="0">$E$1-C4</f>
+        <v>6769.6554999999998</v>
+      </c>
+      <c r="C4" s="1">
+        <v>13.2845</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <f t="shared" si="0"/>
+        <v>6716.2149999999992</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1.6E-2</v>
+      </c>
+      <c r="C5" s="2">
+        <v>66.724999999999994</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <f t="shared" si="0"/>
+        <v>6714.1879999999992</v>
+      </c>
+      <c r="C6" s="1">
+        <v>68.751999999999995</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <f t="shared" si="0"/>
+        <v>6429.24</v>
+      </c>
+      <c r="C7" s="1">
+        <v>353.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <f t="shared" si="0"/>
+        <v>6418.91</v>
+      </c>
+      <c r="B8" s="3">
+        <v>1.78E-2</v>
+      </c>
+      <c r="C8" s="2">
+        <v>364.03</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <f t="shared" si="0"/>
+        <v>6390.4699999999993</v>
+      </c>
+      <c r="B9" s="3">
+        <v>2.9899999999999999E-2</v>
+      </c>
+      <c r="C9" s="2">
+        <v>392.47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <f t="shared" si="0"/>
+        <v>6283.87</v>
+      </c>
+      <c r="C10" s="1">
+        <v>499.07</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <f t="shared" si="0"/>
+        <v>6281.45</v>
+      </c>
+      <c r="C11" s="1">
+        <v>501.49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <f t="shared" si="0"/>
+        <v>6231.94</v>
+      </c>
+      <c r="C12" s="1">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <f t="shared" si="0"/>
+        <v>6228.03</v>
+      </c>
+      <c r="C13" s="1">
+        <v>554.91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <f t="shared" si="0"/>
+        <v>6185.2999999999993</v>
+      </c>
+      <c r="C14" s="1">
+        <v>597.64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <f t="shared" si="0"/>
+        <v>6143.94</v>
+      </c>
+      <c r="C15" s="1">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <f t="shared" si="0"/>
+        <v>6123.95</v>
+      </c>
+      <c r="C16" s="1">
+        <v>658.99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <f t="shared" si="0"/>
+        <v>6041.3399999999992</v>
+      </c>
+      <c r="C17" s="1">
+        <v>741.6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <f t="shared" si="0"/>
+        <v>6006.28</v>
+      </c>
+      <c r="C18" s="1">
+        <v>776.66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <f t="shared" si="0"/>
+        <v>5973.94</v>
+      </c>
+      <c r="C19" s="1">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <f t="shared" si="0"/>
+        <v>5962.94</v>
+      </c>
+      <c r="C20" s="1">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <f t="shared" si="0"/>
+        <v>5957.1399999999994</v>
+      </c>
+      <c r="C21" s="1">
+        <v>825.8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <f t="shared" si="0"/>
+        <v>5914.92</v>
+      </c>
+      <c r="C22" s="1">
+        <v>868.02</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <f t="shared" si="0"/>
+        <v>5888.8399999999992</v>
+      </c>
+      <c r="C23" s="1">
+        <v>894.1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <f t="shared" si="0"/>
+        <v>5878.94</v>
+      </c>
+      <c r="C24" s="1">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <f t="shared" si="0"/>
+        <v>5876.24</v>
+      </c>
+      <c r="C25" s="1">
+        <v>906.7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <f t="shared" si="0"/>
+        <v>5867.49</v>
+      </c>
+      <c r="C26" s="1">
+        <v>915.45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <f t="shared" si="0"/>
+        <v>5851.2099999999991</v>
+      </c>
+      <c r="C27" s="1">
+        <v>931.73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <f t="shared" si="0"/>
+        <v>5789.24</v>
+      </c>
+      <c r="C28" s="1">
+        <v>993.7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <f t="shared" si="0"/>
+        <v>5772.8399999999992</v>
+      </c>
+      <c r="C29" s="1">
+        <v>1010.1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <f t="shared" si="0"/>
+        <v>5755.94</v>
+      </c>
+      <c r="C30" s="1">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <f t="shared" si="0"/>
+        <v>5743.94</v>
+      </c>
+      <c r="C31" s="1">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="2">
+        <f t="shared" si="0"/>
+        <v>5740.4</v>
+      </c>
+      <c r="B32" s="3">
+        <v>1.5100000000000001E-2</v>
+      </c>
+      <c r="C32" s="2">
+        <v>1042.54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <f t="shared" si="0"/>
+        <v>5652.6399999999994</v>
+      </c>
+      <c r="C33" s="1">
+        <v>1130.3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="2">
+        <f t="shared" si="0"/>
+        <v>5651.34</v>
+      </c>
+      <c r="B34" s="3">
+        <v>1.15E-2</v>
+      </c>
+      <c r="C34" s="2">
+        <v>1131.5999999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <f t="shared" si="0"/>
+        <v>5651.07</v>
+      </c>
+      <c r="C35" s="1">
+        <v>1131.8699999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <f t="shared" si="0"/>
+        <v>5649.94</v>
+      </c>
+      <c r="C36" s="1">
+        <v>1133</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <f t="shared" si="0"/>
+        <v>5630.94</v>
+      </c>
+      <c r="C37" s="1">
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <f t="shared" si="0"/>
+        <v>5606.94</v>
+      </c>
+      <c r="C38" s="1">
+        <v>1176</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <f t="shared" si="0"/>
+        <v>5590.94</v>
+      </c>
+      <c r="C39" s="1">
+        <v>1192</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <f t="shared" si="0"/>
+        <v>5536.94</v>
+      </c>
+      <c r="C40" s="1">
+        <v>1246</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <f t="shared" si="0"/>
+        <v>5522.94</v>
+      </c>
+      <c r="C41" s="1">
+        <v>1260</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="2">
+        <f t="shared" si="0"/>
+        <v>5518.5099999999993</v>
+      </c>
+      <c r="B42" s="3">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="C42" s="2">
+        <v>1264.43</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <f t="shared" si="0"/>
+        <v>5470.24</v>
+      </c>
+      <c r="C43" s="1">
+        <v>1312.7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <f t="shared" si="0"/>
+        <v>5464.94</v>
+      </c>
+      <c r="C44" s="1">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
+        <f t="shared" si="0"/>
+        <v>5443.2099999999991</v>
+      </c>
+      <c r="C45" s="1">
+        <v>1339.73</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
+        <f t="shared" si="0"/>
+        <v>5396.84</v>
+      </c>
+      <c r="C46" s="1">
+        <v>1386.1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
+        <f t="shared" si="0"/>
+        <v>5257.6399999999994</v>
+      </c>
+      <c r="C47" s="1">
+        <v>1525.3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <f t="shared" si="0"/>
+        <v>5254.94</v>
+      </c>
+      <c r="C48" s="1">
+        <v>1528</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <f t="shared" si="0"/>
+        <v>5238.4399999999996</v>
+      </c>
+      <c r="C49" s="1">
+        <v>1544.5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
+        <f t="shared" si="0"/>
+        <v>5183.9399999999996</v>
+      </c>
+      <c r="C50" s="1">
+        <v>1599</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <f t="shared" si="0"/>
+        <v>5172.74</v>
+      </c>
+      <c r="C51" s="1">
+        <v>1610.2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <f t="shared" si="0"/>
+        <v>5158.9399999999996</v>
+      </c>
+      <c r="C52" s="1">
+        <v>1624</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
+        <f t="shared" si="0"/>
+        <v>5149.9399999999996</v>
+      </c>
+      <c r="C53" s="1">
+        <v>1633</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
+        <f t="shared" si="0"/>
+        <v>5123.9399999999996</v>
+      </c>
+      <c r="C54" s="1">
+        <v>1659</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
+        <f t="shared" si="0"/>
+        <v>5040.9399999999996</v>
+      </c>
+      <c r="C55" s="1">
+        <v>1742</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
+        <f t="shared" si="0"/>
+        <v>5025.0399999999991</v>
+      </c>
+      <c r="C56" s="1">
+        <v>1757.9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
+        <f t="shared" si="0"/>
+        <v>4978.9399999999996</v>
+      </c>
+      <c r="C57" s="1">
+        <v>1804</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="1">
+        <f t="shared" si="0"/>
+        <v>4911.33</v>
+      </c>
+      <c r="C58" s="1">
+        <v>1871.61</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="1">
+        <f t="shared" si="0"/>
+        <v>4890.84</v>
+      </c>
+      <c r="C59" s="1">
+        <v>1892.1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="1">
+        <f t="shared" si="0"/>
+        <v>4870.5399999999991</v>
+      </c>
+      <c r="C60" s="1">
+        <v>1912.4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="1">
+        <f t="shared" si="0"/>
+        <v>4851.74</v>
+      </c>
+      <c r="C61" s="1">
+        <v>1931.2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="1">
+        <f t="shared" si="0"/>
+        <v>4820.9399999999996</v>
+      </c>
+      <c r="C62" s="1">
+        <v>1962</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="1">
+        <f t="shared" si="0"/>
+        <v>4788.74</v>
+      </c>
+      <c r="C63" s="1">
+        <v>1994.2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" s="1">
+        <f t="shared" si="0"/>
+        <v>4779.24</v>
+      </c>
+      <c r="C64" s="1">
+        <v>2003.7</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" s="1">
+        <f t="shared" si="0"/>
+        <v>4779.1399999999994</v>
+      </c>
+      <c r="C65" s="1">
+        <v>2003.8</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" s="1">
+        <f t="shared" si="0"/>
+        <v>4744.84</v>
+      </c>
+      <c r="C66" s="1">
+        <v>2038.1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" s="1">
+        <f t="shared" si="0"/>
+        <v>4716.9399999999996</v>
+      </c>
+      <c r="C67" s="1">
+        <v>2066</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" s="1">
+        <f t="shared" ref="A68:A131" si="1">$E$1-C68</f>
+        <v>4694.9399999999996</v>
+      </c>
+      <c r="C68" s="1">
+        <v>2088</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" s="1">
+        <f t="shared" si="1"/>
+        <v>4681.74</v>
+      </c>
+      <c r="C69" s="1">
+        <v>2101.1999999999998</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" s="1">
+        <f t="shared" si="1"/>
+        <v>4650.84</v>
+      </c>
+      <c r="C70" s="1">
+        <v>2132.1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" s="1">
+        <f t="shared" si="1"/>
+        <v>4641.4399999999996</v>
+      </c>
+      <c r="C71" s="1">
+        <v>2141.5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="1">
+        <f t="shared" si="1"/>
+        <v>4618.9399999999996</v>
+      </c>
+      <c r="C72" s="1">
+        <v>2164</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" s="1">
+        <f t="shared" si="1"/>
+        <v>4594.24</v>
+      </c>
+      <c r="C73" s="1">
+        <v>2188.6999999999998</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" s="1">
+        <f t="shared" si="1"/>
+        <v>4572.4399999999996</v>
+      </c>
+      <c r="C74" s="1">
+        <v>2210.5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" s="1">
+        <f t="shared" si="1"/>
+        <v>4565.84</v>
+      </c>
+      <c r="C75" s="1">
+        <v>2217.1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" s="1">
+        <f t="shared" si="1"/>
+        <v>4515.9399999999996</v>
+      </c>
+      <c r="C76" s="1">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" s="1">
+        <f t="shared" si="1"/>
+        <v>4492.1399999999994</v>
+      </c>
+      <c r="C77" s="1">
+        <v>2290.8000000000002</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" s="1">
+        <f t="shared" si="1"/>
+        <v>4470.9399999999996</v>
+      </c>
+      <c r="C78" s="1">
+        <v>2312</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" s="1">
+        <f t="shared" si="1"/>
+        <v>4463.6399999999994</v>
+      </c>
+      <c r="C79" s="1">
+        <v>2319.3000000000002</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" s="1">
+        <f t="shared" si="1"/>
+        <v>4447.9399999999996</v>
+      </c>
+      <c r="C80" s="1">
+        <v>2335</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" s="1">
+        <f t="shared" si="1"/>
+        <v>4422.9399999999996</v>
+      </c>
+      <c r="C81" s="1">
+        <v>2360</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" s="1">
+        <f t="shared" si="1"/>
+        <v>4421.84</v>
+      </c>
+      <c r="C82" s="1">
+        <v>2361.1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83" s="1">
+        <f t="shared" si="1"/>
+        <v>4408.9399999999996</v>
+      </c>
+      <c r="C83" s="1">
+        <v>2374</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" s="1">
+        <f t="shared" si="1"/>
+        <v>4381.34</v>
+      </c>
+      <c r="C84" s="1">
+        <v>2401.6</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85" s="1">
+        <f t="shared" si="1"/>
+        <v>4363.6399999999994</v>
+      </c>
+      <c r="C85" s="1">
+        <v>2419.3000000000002</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" s="1">
+        <f t="shared" si="1"/>
+        <v>4328.9399999999996</v>
+      </c>
+      <c r="C86" s="1">
+        <v>2454</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" s="1">
+        <f t="shared" si="1"/>
+        <v>4323.9399999999996</v>
+      </c>
+      <c r="C87" s="1">
+        <v>2459</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" s="1">
+        <f t="shared" si="1"/>
+        <v>4312.9399999999996</v>
+      </c>
+      <c r="C88" s="1">
+        <v>2470</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89" s="1">
+        <f t="shared" si="1"/>
+        <v>4299.4399999999996</v>
+      </c>
+      <c r="C89" s="1">
+        <v>2483.5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" s="1">
+        <f t="shared" si="1"/>
+        <v>4274.9399999999996</v>
+      </c>
+      <c r="C90" s="1">
+        <v>2508</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91" s="1">
+        <f t="shared" si="1"/>
+        <v>4218.0399999999991</v>
+      </c>
+      <c r="C91" s="1">
+        <v>2564.9</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92" s="1">
+        <f t="shared" si="1"/>
+        <v>4206.9399999999996</v>
+      </c>
+      <c r="C92" s="1">
+        <v>2576</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93" s="1">
+        <f t="shared" si="1"/>
+        <v>4164.9399999999996</v>
+      </c>
+      <c r="C93" s="1">
+        <v>2618</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94" s="1">
+        <f t="shared" si="1"/>
+        <v>4104.9399999999996</v>
+      </c>
+      <c r="C94" s="1">
+        <v>2678</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A95" s="1">
+        <f t="shared" si="1"/>
+        <v>4086.9399999999996</v>
+      </c>
+      <c r="C95" s="1">
+        <v>2696</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A96" s="1">
+        <f t="shared" si="1"/>
+        <v>4076.5399999999995</v>
+      </c>
+      <c r="C96" s="1">
+        <v>2706.4</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A97" s="1">
+        <f t="shared" si="1"/>
+        <v>4062.4399999999996</v>
+      </c>
+      <c r="C97" s="1">
+        <v>2720.5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98" s="1">
+        <f t="shared" si="1"/>
+        <v>4050.9399999999996</v>
+      </c>
+      <c r="C98" s="1">
+        <v>2732</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A99" s="1">
+        <f t="shared" si="1"/>
+        <v>4039.9399999999996</v>
+      </c>
+      <c r="C99" s="1">
+        <v>2743</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A100" s="1">
+        <f t="shared" si="1"/>
+        <v>4022.4399999999996</v>
+      </c>
+      <c r="C100" s="1">
+        <v>2760.5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A101" s="1">
+        <f t="shared" si="1"/>
+        <v>4008.1399999999994</v>
+      </c>
+      <c r="C101" s="1">
+        <v>2774.8</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A102" s="1">
+        <f t="shared" si="1"/>
+        <v>3986.9399999999996</v>
+      </c>
+      <c r="C102" s="1">
+        <v>2796</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A103" s="1">
+        <f t="shared" si="1"/>
+        <v>3967.9399999999996</v>
+      </c>
+      <c r="C103" s="1">
+        <v>2815</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A104" s="1">
+        <f t="shared" si="1"/>
+        <v>3946.9399999999996</v>
+      </c>
+      <c r="C104" s="1">
+        <v>2836</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A105" s="1">
+        <f t="shared" si="1"/>
+        <v>3898.4399999999996</v>
+      </c>
+      <c r="C105" s="1">
+        <v>2884.5</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A106" s="1">
+        <f t="shared" si="1"/>
+        <v>3867.9399999999996</v>
+      </c>
+      <c r="C106" s="1">
+        <v>2915</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A107" s="1">
+        <f t="shared" si="1"/>
+        <v>3852.4399999999996</v>
+      </c>
+      <c r="C107" s="1">
+        <v>2930.5</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A108" s="1">
+        <f t="shared" si="1"/>
+        <v>3809.9399999999996</v>
+      </c>
+      <c r="C108" s="1">
+        <v>2973</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A109" s="1">
+        <f t="shared" si="1"/>
+        <v>3776.1399999999994</v>
+      </c>
+      <c r="C109" s="1">
+        <v>3006.8</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A110" s="1">
+        <f t="shared" si="1"/>
+        <v>3765.9399999999996</v>
+      </c>
+      <c r="C110" s="1">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A111" s="1">
+        <f t="shared" si="1"/>
+        <v>3745.9399999999996</v>
+      </c>
+      <c r="C111" s="1">
+        <v>3037</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A112" s="1">
+        <f t="shared" si="1"/>
+        <v>3724.9399999999996</v>
+      </c>
+      <c r="C112" s="1">
+        <v>3058</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A113" s="1">
+        <f t="shared" si="1"/>
+        <v>3610.9399999999996</v>
+      </c>
+      <c r="C113" s="1">
+        <v>3172</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A114" s="1">
+        <f t="shared" si="1"/>
+        <v>3601.8399999999997</v>
+      </c>
+      <c r="C114" s="1">
+        <v>3181.1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A115" s="1">
+        <f t="shared" si="1"/>
+        <v>3583.5399999999995</v>
+      </c>
+      <c r="C115" s="1">
+        <v>3199.4</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A116" s="1">
+        <f t="shared" si="1"/>
+        <v>3560.9399999999996</v>
+      </c>
+      <c r="C116" s="1">
+        <v>3222</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A117" s="1">
+        <f t="shared" si="1"/>
+        <v>3559.9399999999996</v>
+      </c>
+      <c r="C117" s="1">
+        <v>3223</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A118" s="1">
+        <f t="shared" si="1"/>
+        <v>3505.9399999999996</v>
+      </c>
+      <c r="C118" s="1">
+        <v>3277</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A119" s="1">
+        <f t="shared" si="1"/>
+        <v>3477.9399999999996</v>
+      </c>
+      <c r="C119" s="1">
+        <v>3305</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A120" s="1">
+        <f t="shared" si="1"/>
+        <v>3426.9399999999996</v>
+      </c>
+      <c r="C120" s="1">
+        <v>3356</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A121" s="1">
+        <f t="shared" si="1"/>
+        <v>3398.9399999999996</v>
+      </c>
+      <c r="C121" s="1">
+        <v>3384</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A122" s="1">
+        <f t="shared" si="1"/>
+        <v>3364.9399999999996</v>
+      </c>
+      <c r="C122" s="1">
+        <v>3418</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A123" s="1">
+        <f t="shared" si="1"/>
+        <v>3268.9399999999996</v>
+      </c>
+      <c r="C123" s="1">
+        <v>3514</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A124" s="1">
+        <f t="shared" si="1"/>
+        <v>3231.9399999999996</v>
+      </c>
+      <c r="C124" s="1">
+        <v>3551</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A125" s="1">
+        <f t="shared" si="1"/>
+        <v>3159.9399999999996</v>
+      </c>
+      <c r="C125" s="1">
+        <v>3623</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A126" s="1">
+        <f t="shared" si="1"/>
+        <v>3151.9399999999996</v>
+      </c>
+      <c r="C126" s="1">
+        <v>3631</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A127" s="1">
+        <f t="shared" si="1"/>
+        <v>3079.9399999999996</v>
+      </c>
+      <c r="C127" s="1">
+        <v>3703</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A128" s="1">
+        <f t="shared" si="1"/>
+        <v>3055.9399999999996</v>
+      </c>
+      <c r="C128" s="1">
+        <v>3727</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A129" s="1">
+        <f t="shared" si="1"/>
+        <v>3016.9399999999996</v>
+      </c>
+      <c r="C129" s="1">
+        <v>3766</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A130" s="1">
+        <f t="shared" si="1"/>
+        <v>2976.9399999999996</v>
+      </c>
+      <c r="C130" s="1">
+        <v>3806</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A131" s="1">
+        <f t="shared" si="1"/>
+        <v>2933.9399999999996</v>
+      </c>
+      <c r="C131" s="1">
+        <v>3849</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A132" s="1">
+        <f t="shared" ref="A132:A145" si="2">$E$1-C132</f>
+        <v>2907.4399999999996</v>
+      </c>
+      <c r="C132" s="1">
+        <v>3875.5</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A133" s="1">
+        <f t="shared" si="2"/>
+        <v>2859.9399999999996</v>
+      </c>
+      <c r="C133" s="1">
+        <v>3923</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A134" s="1">
+        <f t="shared" si="2"/>
+        <v>2837.9399999999996</v>
+      </c>
+      <c r="C134" s="1">
+        <v>3945</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A135" s="1">
+        <f t="shared" si="2"/>
+        <v>2780.9399999999996</v>
+      </c>
+      <c r="C135" s="1">
+        <v>4002</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A136" s="1">
+        <f t="shared" si="2"/>
+        <v>2723.9399999999996</v>
+      </c>
+      <c r="C136" s="1">
+        <v>4059</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A137" s="1">
+        <f t="shared" si="2"/>
+        <v>2709.9399999999996</v>
+      </c>
+      <c r="C137" s="1">
+        <v>4073</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A138" s="1">
+        <f t="shared" si="2"/>
+        <v>2412.9399999999996</v>
+      </c>
+      <c r="C138" s="1">
+        <v>4370</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A139" s="1">
+        <f t="shared" si="2"/>
+        <v>2345.9399999999996</v>
+      </c>
+      <c r="C139" s="1">
+        <v>4437</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A140" s="1">
+        <f t="shared" si="2"/>
+        <v>2213.9399999999996</v>
+      </c>
+      <c r="C140" s="1">
+        <v>4569</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A141" s="1">
+        <f t="shared" si="2"/>
+        <v>2181.9399999999996</v>
+      </c>
+      <c r="C141" s="1">
+        <v>4601</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A142" s="1">
+        <f t="shared" si="2"/>
+        <v>2173.54</v>
+      </c>
+      <c r="C142" s="1">
+        <v>4609.3999999999996</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A143" s="1">
+        <f t="shared" si="2"/>
+        <v>2129.9399999999996</v>
+      </c>
+      <c r="C143" s="1">
+        <v>4653</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A144" s="1">
+        <f t="shared" si="2"/>
+        <v>2115.9399999999996</v>
+      </c>
+      <c r="C144" s="1">
+        <v>4667</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A145" s="1">
+        <f t="shared" si="2"/>
+        <v>-1.0000000000218279E-2</v>
+      </c>
+      <c r="C145" s="1">
+        <v>6782.95</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A146" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B146" s="4">
+        <f>SUM(B3:B145)</f>
+        <v>0.11929999999999999</v>
+      </c>
+      <c r="C146" s="5">
+        <f>(B146/G1)*100</f>
+        <v>5.1869565217391305</v>
+      </c>
+      <c r="D146" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E239AF0B-EC93-E840-8919-26D601FE4BD8}">
+  <dimension ref="A1:G136"/>
+  <sheetViews>
+    <sheetView topLeftCell="A117" workbookViewId="0">
+      <selection activeCell="B142" sqref="B142"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.83203125" customWidth="1"/>
+    <col min="2" max="3" width="21.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1">
+        <f>isotopes!F5*1000</f>
+        <v>6505.84</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <f>$E$1-C3</f>
+        <v>6505.84</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <f t="shared" ref="A4:B67" si="0">$E$1-C4</f>
+        <v>6443.92</v>
+      </c>
+      <c r="C4">
+        <v>61.92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <f t="shared" si="0"/>
+        <v>6366.1500000000005</v>
+      </c>
+      <c r="C5">
+        <v>139.69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <f t="shared" si="0"/>
+        <v>6313.6500000000005</v>
+      </c>
+      <c r="C6">
+        <v>192.19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <f t="shared" si="0"/>
+        <v>6305.95</v>
+      </c>
+      <c r="C7">
+        <v>199.89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <f t="shared" si="0"/>
+        <v>6252.6900000000005</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1.8800000000000001E-2</v>
+      </c>
+      <c r="C8" s="3">
+        <v>253.15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <f t="shared" si="0"/>
+        <v>6189.03</v>
+      </c>
+      <c r="C9">
+        <v>316.81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <f t="shared" si="0"/>
+        <v>6048.77</v>
+      </c>
+      <c r="C10">
+        <v>457.07</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <f t="shared" si="0"/>
+        <v>5931.14</v>
+      </c>
+      <c r="C11">
+        <v>574.70000000000005</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <f t="shared" si="0"/>
+        <v>5921.42</v>
+      </c>
+      <c r="C12">
+        <v>584.41999999999996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <f t="shared" si="0"/>
+        <v>5854.84</v>
+      </c>
+      <c r="C13">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <f t="shared" si="0"/>
+        <v>5832.17</v>
+      </c>
+      <c r="C14">
+        <v>673.67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <f t="shared" si="0"/>
+        <v>5746.34</v>
+      </c>
+      <c r="C15">
+        <v>759.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <f t="shared" si="0"/>
+        <v>5743.64</v>
+      </c>
+      <c r="C16">
+        <v>762.2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <f t="shared" si="0"/>
+        <v>5675.84</v>
+      </c>
+      <c r="C17">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <f t="shared" si="0"/>
+        <v>5620.37</v>
+      </c>
+      <c r="C18">
+        <v>885.47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <f t="shared" si="0"/>
+        <v>5603.9400000000005</v>
+      </c>
+      <c r="C19">
+        <v>901.9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <f t="shared" si="0"/>
+        <v>5559.4400000000005</v>
+      </c>
+      <c r="C20">
+        <v>946.4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <f t="shared" si="0"/>
+        <v>5519.04</v>
+      </c>
+      <c r="C21">
+        <v>986.8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <f t="shared" si="0"/>
+        <v>5443.64</v>
+      </c>
+      <c r="C22">
+        <v>1062.2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <f t="shared" si="0"/>
+        <v>5424.84</v>
+      </c>
+      <c r="C23">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <f t="shared" si="0"/>
+        <v>5378.04</v>
+      </c>
+      <c r="C24">
+        <v>1127.8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <f t="shared" si="0"/>
+        <v>5368.91</v>
+      </c>
+      <c r="C25">
+        <v>1136.93</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <f t="shared" si="0"/>
+        <v>5315.84</v>
+      </c>
+      <c r="C26">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <f t="shared" si="0"/>
+        <v>5283.64</v>
+      </c>
+      <c r="C27">
+        <v>1222.2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <f t="shared" si="0"/>
+        <v>5265.09</v>
+      </c>
+      <c r="C28">
+        <v>1240.75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <f t="shared" si="0"/>
+        <v>5248.84</v>
+      </c>
+      <c r="C29">
+        <v>1257</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <f t="shared" si="0"/>
+        <v>5171.04</v>
+      </c>
+      <c r="C30">
+        <v>1334.8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <f t="shared" si="0"/>
+        <v>5111.43</v>
+      </c>
+      <c r="C31">
+        <v>1394.41</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <f t="shared" si="0"/>
+        <v>5100.34</v>
+      </c>
+      <c r="C32">
+        <v>1405.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <f t="shared" si="0"/>
+        <v>5089.63</v>
+      </c>
+      <c r="C33">
+        <v>1416.21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <f t="shared" si="0"/>
+        <v>5077.63</v>
+      </c>
+      <c r="C34">
+        <v>1428.21</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <f t="shared" si="0"/>
+        <v>5010.9400000000005</v>
+      </c>
+      <c r="C35">
+        <v>1494.9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <f t="shared" si="0"/>
+        <v>5004.2800000000007</v>
+      </c>
+      <c r="C36">
+        <v>1501.56</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <f t="shared" si="0"/>
+        <v>5003.8</v>
+      </c>
+      <c r="C37">
+        <v>1502.04</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <f t="shared" si="0"/>
+        <v>4991.38</v>
+      </c>
+      <c r="C38">
+        <v>1514.46</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <f t="shared" si="0"/>
+        <v>4968.1400000000003</v>
+      </c>
+      <c r="C39">
+        <v>1537.7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <f t="shared" si="0"/>
+        <v>4903.04</v>
+      </c>
+      <c r="C40">
+        <v>1602.8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <f t="shared" si="0"/>
+        <v>4823.84</v>
+      </c>
+      <c r="C41">
+        <v>1682</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <f t="shared" si="0"/>
+        <v>4817.74</v>
+      </c>
+      <c r="C42">
+        <v>1688.1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <f t="shared" si="0"/>
+        <v>4809.84</v>
+      </c>
+      <c r="C43">
+        <v>1696</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <f t="shared" si="0"/>
+        <v>4787.3500000000004</v>
+      </c>
+      <c r="C44">
+        <v>1718.49</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
+        <f t="shared" si="0"/>
+        <v>4748.21</v>
+      </c>
+      <c r="C45">
+        <v>1757.63</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
+        <f t="shared" si="0"/>
+        <v>4709.54</v>
+      </c>
+      <c r="C46">
+        <v>1796.3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
+        <f t="shared" si="0"/>
+        <v>4636.41</v>
+      </c>
+      <c r="C47">
+        <v>1869.43</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <f t="shared" si="0"/>
+        <v>4604.84</v>
+      </c>
+      <c r="C48">
+        <v>1901</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <f t="shared" si="0"/>
+        <v>4501.95</v>
+      </c>
+      <c r="C49">
+        <v>2003.89</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
+        <f t="shared" si="0"/>
+        <v>4451.84</v>
+      </c>
+      <c r="C50">
+        <v>2054</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <f t="shared" si="0"/>
+        <v>4440.34</v>
+      </c>
+      <c r="C51">
+        <v>2065.5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <f t="shared" si="0"/>
+        <v>4414.8099999999995</v>
+      </c>
+      <c r="C52">
+        <v>2091.0300000000002</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
+        <f t="shared" si="0"/>
+        <v>4402.1100000000006</v>
+      </c>
+      <c r="C53">
+        <v>2103.73</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
+        <f t="shared" si="0"/>
+        <v>4395.74</v>
+      </c>
+      <c r="C54">
+        <v>2110.1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
+        <f t="shared" si="0"/>
+        <v>4378.84</v>
+      </c>
+      <c r="C55">
+        <v>2127</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
+        <f t="shared" si="0"/>
+        <v>4354.84</v>
+      </c>
+      <c r="C56">
+        <v>2151</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
+        <f t="shared" si="0"/>
+        <v>4308.74</v>
+      </c>
+      <c r="C57">
+        <v>2197.1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="1">
+        <f t="shared" si="0"/>
+        <v>4291.04</v>
+      </c>
+      <c r="C58">
+        <v>2214.8000000000002</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="1">
+        <f t="shared" si="0"/>
+        <v>4224.84</v>
+      </c>
+      <c r="C59">
+        <v>2281</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="1">
+        <f t="shared" si="0"/>
+        <v>4194.21</v>
+      </c>
+      <c r="C60">
+        <v>2311.63</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="1">
+        <f t="shared" si="0"/>
+        <v>4185.84</v>
+      </c>
+      <c r="C61">
+        <v>2320</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="1">
+        <f t="shared" si="0"/>
+        <v>4184.84</v>
+      </c>
+      <c r="C62">
+        <v>2321</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="1">
+        <f t="shared" si="0"/>
+        <v>4146.84</v>
+      </c>
+      <c r="C63">
+        <v>2359</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" s="1">
+        <f t="shared" si="0"/>
+        <v>4122.96</v>
+      </c>
+      <c r="C64">
+        <v>2382.88</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" s="1">
+        <f t="shared" si="0"/>
+        <v>4121.84</v>
+      </c>
+      <c r="C65">
+        <v>2384</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" s="1">
+        <f t="shared" si="0"/>
+        <v>4027.84</v>
+      </c>
+      <c r="C66">
+        <v>2478</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" s="1">
+        <f t="shared" si="0"/>
+        <v>4011.94</v>
+      </c>
+      <c r="C67">
+        <v>2493.9</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" s="1">
+        <f t="shared" ref="A68:A131" si="1">$E$1-C68</f>
+        <v>3978.57</v>
+      </c>
+      <c r="C68">
+        <v>2527.27</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" s="1">
+        <f t="shared" si="1"/>
+        <v>3971.84</v>
+      </c>
+      <c r="C69">
+        <v>2534</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" s="1">
+        <f t="shared" si="1"/>
+        <v>3961.44</v>
+      </c>
+      <c r="C70">
+        <v>2544.4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" s="1">
+        <f t="shared" si="1"/>
+        <v>3935.54</v>
+      </c>
+      <c r="C71">
+        <v>2570.3000000000002</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="1">
+        <f t="shared" si="1"/>
+        <v>3931.6400000000003</v>
+      </c>
+      <c r="C72">
+        <v>2574.1999999999998</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" s="1">
+        <f t="shared" si="1"/>
+        <v>3845.09</v>
+      </c>
+      <c r="C73">
+        <v>2660.75</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" s="1">
+        <f t="shared" si="1"/>
+        <v>3841.4100000000003</v>
+      </c>
+      <c r="C74">
+        <v>2664.43</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" s="1">
+        <f t="shared" si="1"/>
+        <v>3840.7400000000002</v>
+      </c>
+      <c r="C75">
+        <v>2665.1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" s="1">
+        <f t="shared" si="1"/>
+        <v>3826.2400000000002</v>
+      </c>
+      <c r="C76">
+        <v>2679.6</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" s="1">
+        <f t="shared" si="1"/>
+        <v>3765.84</v>
+      </c>
+      <c r="C77">
+        <v>2740</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" s="1">
+        <f t="shared" si="1"/>
+        <v>3761.6400000000003</v>
+      </c>
+      <c r="C78">
+        <v>2744.2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" s="1">
+        <f t="shared" si="1"/>
+        <v>3757.34</v>
+      </c>
+      <c r="C79">
+        <v>2748.5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" s="1">
+        <f t="shared" si="1"/>
+        <v>3748.54</v>
+      </c>
+      <c r="C80">
+        <v>2757.3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" s="1">
+        <f t="shared" si="1"/>
+        <v>3746.6400000000003</v>
+      </c>
+      <c r="C81">
+        <v>2759.2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" s="1">
+        <f t="shared" si="1"/>
+        <v>3724.84</v>
+      </c>
+      <c r="C82">
+        <v>2781</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83" s="1">
+        <f t="shared" si="1"/>
+        <v>3721.94</v>
+      </c>
+      <c r="C83">
+        <v>2783.9</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" s="1">
+        <f t="shared" si="1"/>
+        <v>3670.84</v>
+      </c>
+      <c r="C84">
+        <v>2835</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85" s="1">
+        <f t="shared" si="1"/>
+        <v>3669.84</v>
+      </c>
+      <c r="C85">
+        <v>2836</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" s="1">
+        <f t="shared" si="1"/>
+        <v>3665.84</v>
+      </c>
+      <c r="C86">
+        <v>2840</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" s="1">
+        <f t="shared" si="1"/>
+        <v>3653.04</v>
+      </c>
+      <c r="C87">
+        <v>2852.8</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" s="1">
+        <f t="shared" si="1"/>
+        <v>3639.84</v>
+      </c>
+      <c r="C88">
+        <v>2866</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89" s="1">
+        <f t="shared" si="1"/>
+        <v>3608.44</v>
+      </c>
+      <c r="C89">
+        <v>2897.4</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" s="1">
+        <f t="shared" si="1"/>
+        <v>3577.54</v>
+      </c>
+      <c r="C90">
+        <v>2928.3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91" s="1">
+        <f t="shared" si="1"/>
+        <v>3566.84</v>
+      </c>
+      <c r="C91">
+        <v>2939</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92" s="1">
+        <f t="shared" si="1"/>
+        <v>3553.34</v>
+      </c>
+      <c r="C92">
+        <v>2952.5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93" s="1">
+        <f t="shared" si="1"/>
+        <v>3541.44</v>
+      </c>
+      <c r="C93">
+        <v>2964.4</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94" s="1">
+        <f t="shared" si="1"/>
+        <v>3510.94</v>
+      </c>
+      <c r="C94">
+        <v>2994.9</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A95" s="1">
+        <f t="shared" si="1"/>
+        <v>3501.6400000000003</v>
+      </c>
+      <c r="C95">
+        <v>3004.2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A96" s="1">
+        <f t="shared" si="1"/>
+        <v>3474.1400000000003</v>
+      </c>
+      <c r="C96">
+        <v>3031.7</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A97" s="1">
+        <f t="shared" si="1"/>
+        <v>3463.84</v>
+      </c>
+      <c r="C97">
+        <v>3042</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98" s="1">
+        <f t="shared" si="1"/>
+        <v>3457.1400000000003</v>
+      </c>
+      <c r="C98">
+        <v>3048.7</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A99" s="1">
+        <f t="shared" si="1"/>
+        <v>3438.44</v>
+      </c>
+      <c r="C99">
+        <v>3067.4</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A100" s="1">
+        <f t="shared" si="1"/>
+        <v>3423.54</v>
+      </c>
+      <c r="C100">
+        <v>3082.3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A101" s="1">
+        <f t="shared" si="1"/>
+        <v>3413.84</v>
+      </c>
+      <c r="C101">
+        <v>3092</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A102" s="1">
+        <f t="shared" si="1"/>
+        <v>3379.84</v>
+      </c>
+      <c r="C102">
+        <v>3126</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A103" s="1">
+        <f t="shared" si="1"/>
+        <v>3369.84</v>
+      </c>
+      <c r="C103">
+        <v>3136</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A104" s="1">
+        <f t="shared" si="1"/>
+        <v>3343.34</v>
+      </c>
+      <c r="C104">
+        <v>3162.5</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A105" s="1">
+        <f t="shared" si="1"/>
+        <v>3335.44</v>
+      </c>
+      <c r="C105">
+        <v>3170.4</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A106" s="1">
+        <f t="shared" si="1"/>
+        <v>3303.84</v>
+      </c>
+      <c r="C106">
+        <v>3202</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A107" s="1">
+        <f t="shared" si="1"/>
+        <v>3291.84</v>
+      </c>
+      <c r="C107">
+        <v>3214</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A108" s="1">
+        <f t="shared" si="1"/>
+        <v>3279.34</v>
+      </c>
+      <c r="C108">
+        <v>3226.5</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A109" s="1">
+        <f t="shared" si="1"/>
+        <v>3226.2400000000002</v>
+      </c>
+      <c r="C109">
+        <v>3279.6</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A110" s="1">
+        <f t="shared" si="1"/>
+        <v>3215.84</v>
+      </c>
+      <c r="C110">
+        <v>3290</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A111" s="1">
+        <f t="shared" si="1"/>
+        <v>3144.84</v>
+      </c>
+      <c r="C111">
+        <v>3361</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A112" s="1">
+        <f t="shared" si="1"/>
+        <v>3135.84</v>
+      </c>
+      <c r="C112">
+        <v>3370</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A113" s="1">
+        <f t="shared" si="1"/>
+        <v>3112.84</v>
+      </c>
+      <c r="C113">
+        <v>3393</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A114" s="1">
+        <f t="shared" si="1"/>
+        <v>3067.84</v>
+      </c>
+      <c r="C114">
+        <v>3438</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A115" s="1">
+        <f t="shared" si="1"/>
+        <v>3055.84</v>
+      </c>
+      <c r="C115">
+        <v>3450</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A116" s="1">
+        <f t="shared" si="1"/>
+        <v>3011.84</v>
+      </c>
+      <c r="C116">
+        <v>3494</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A117" s="1">
+        <f t="shared" si="1"/>
+        <v>2973.84</v>
+      </c>
+      <c r="C117">
+        <v>3532</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A118" s="1">
+        <f t="shared" si="1"/>
+        <v>2945.84</v>
+      </c>
+      <c r="C118">
+        <v>3560</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A119" s="1">
+        <f t="shared" si="1"/>
+        <v>2879.84</v>
+      </c>
+      <c r="C119">
+        <v>3626</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A120" s="1">
+        <f t="shared" si="1"/>
+        <v>2786.84</v>
+      </c>
+      <c r="C120">
+        <v>3719</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A121" s="1">
+        <f t="shared" si="1"/>
+        <v>2746.84</v>
+      </c>
+      <c r="C121">
+        <v>3759</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A122" s="1">
+        <f t="shared" si="1"/>
+        <v>2693.84</v>
+      </c>
+      <c r="C122">
+        <v>3812</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A123" s="1">
+        <f t="shared" si="1"/>
+        <v>2666.84</v>
+      </c>
+      <c r="C123">
+        <v>3839</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A124" s="1">
+        <f t="shared" si="1"/>
+        <v>2643.84</v>
+      </c>
+      <c r="C124">
+        <v>3862</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A125" s="1">
+        <f t="shared" si="1"/>
+        <v>0.23999999999978172</v>
+      </c>
+      <c r="C125">
+        <v>6505.6</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A126" s="1">
+        <f t="shared" si="1"/>
+        <v>-2.2899999999999636</v>
+      </c>
+      <c r="C126">
+        <v>6508.13</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A127" s="1">
+        <f t="shared" si="1"/>
+        <v>-2.4799999999995634</v>
+      </c>
+      <c r="C127">
+        <v>6508.32</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A128" s="1">
+        <f t="shared" si="1"/>
+        <v>-3.5799999999999272</v>
+      </c>
+      <c r="C128">
+        <v>6509.42</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A129" s="1">
+        <f t="shared" si="1"/>
+        <v>-4.430000000000291</v>
+      </c>
+      <c r="C129">
+        <v>6510.27</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A130" s="1">
+        <f t="shared" si="1"/>
+        <v>-11.389999999999418</v>
+      </c>
+      <c r="C130">
+        <v>6517.23</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A131" s="1">
+        <f t="shared" si="1"/>
+        <v>-18.789999999999964</v>
+      </c>
+      <c r="C131">
+        <v>6524.63</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A132" s="1">
+        <f t="shared" ref="A132:A135" si="2">$E$1-C132</f>
+        <v>-21.1899999999996</v>
+      </c>
+      <c r="C132">
+        <v>6527.03</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A133" s="1">
+        <f t="shared" si="2"/>
+        <v>-23.859999999999673</v>
+      </c>
+      <c r="C133">
+        <v>6529.7</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A134" s="1">
+        <f t="shared" si="2"/>
+        <v>-42.059999999999491</v>
+      </c>
+      <c r="C134">
+        <v>6547.9</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A135" s="1">
+        <f t="shared" si="2"/>
+        <v>-59.859999999999673</v>
+      </c>
+      <c r="C135">
+        <v>6565.7</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A136" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B136" s="4">
+        <f>SUM(B3:B135)</f>
+        <v>1.8800000000000001E-2</v>
+      </c>
+      <c r="C136" s="5">
+        <f>(B136/G1)*100</f>
+        <v>0.81739130434782625</v>
+      </c>
+      <c r="D136" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A4804E8-4BFC-6547-923C-4185BBF38699}">
+  <dimension ref="A1:G76"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C77" sqref="C77"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="2" max="3" width="21.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1">
+        <f>isotopes!F6*1000</f>
+        <v>6071.29</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <f>$E$1-C3</f>
+        <v>6071.29</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <f t="shared" ref="A4:A67" si="0">$E$1-C4</f>
+        <v>5911.58</v>
+      </c>
+      <c r="C4">
+        <v>159.71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <f t="shared" si="0"/>
+        <v>5846.33</v>
+      </c>
+      <c r="C5">
+        <v>224.96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <f t="shared" si="0"/>
+        <v>5649.9</v>
+      </c>
+      <c r="C6">
+        <v>421.39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <f t="shared" si="0"/>
+        <v>5579.24</v>
+      </c>
+      <c r="C7">
+        <v>492.05</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <f t="shared" si="0"/>
+        <v>5566.53</v>
+      </c>
+      <c r="C8">
+        <v>504.76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <f t="shared" si="0"/>
+        <v>5452.43</v>
+      </c>
+      <c r="C9">
+        <v>618.86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <f t="shared" si="0"/>
+        <v>5441.61</v>
+      </c>
+      <c r="C10">
+        <v>629.67999999999995</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <f t="shared" si="0"/>
+        <v>5310.76</v>
+      </c>
+      <c r="C11">
+        <v>760.53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <f t="shared" si="0"/>
+        <v>5262.2</v>
+      </c>
+      <c r="C12">
+        <v>809.09</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <f t="shared" si="0"/>
+        <v>5187.1000000000004</v>
+      </c>
+      <c r="C13">
+        <v>884.19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <f t="shared" si="0"/>
+        <v>5160.68</v>
+      </c>
+      <c r="C14">
+        <v>910.61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <f t="shared" si="0"/>
+        <v>5049.71</v>
+      </c>
+      <c r="C15">
+        <v>1021.58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <f t="shared" si="0"/>
+        <v>5023.24</v>
+      </c>
+      <c r="C16">
+        <v>1048.05</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <f t="shared" si="0"/>
+        <v>5018.5599999999995</v>
+      </c>
+      <c r="C17">
+        <v>1052.73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <f t="shared" si="0"/>
+        <v>4960.6099999999997</v>
+      </c>
+      <c r="C18">
+        <v>1110.68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <f t="shared" si="0"/>
+        <v>4882.29</v>
+      </c>
+      <c r="C19">
+        <v>1189</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <f t="shared" si="0"/>
+        <v>4824.29</v>
+      </c>
+      <c r="C20">
+        <v>1247</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <f t="shared" si="0"/>
+        <v>4795.88</v>
+      </c>
+      <c r="C21">
+        <v>1275.4100000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <f t="shared" si="0"/>
+        <v>4784.76</v>
+      </c>
+      <c r="C22">
+        <v>1286.53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <f t="shared" si="0"/>
+        <v>4726.62</v>
+      </c>
+      <c r="C23">
+        <v>1344.67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <f t="shared" si="0"/>
+        <v>4712.21</v>
+      </c>
+      <c r="C24">
+        <v>1359.08</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <f t="shared" si="0"/>
+        <v>4686.01</v>
+      </c>
+      <c r="C25">
+        <v>1385.28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <f t="shared" si="0"/>
+        <v>4662.83</v>
+      </c>
+      <c r="C26">
+        <v>1408.46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <f t="shared" si="0"/>
+        <v>4536.01</v>
+      </c>
+      <c r="C27">
+        <v>1535.28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <f t="shared" si="0"/>
+        <v>4461.29</v>
+      </c>
+      <c r="C28">
+        <v>1610</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <f t="shared" si="0"/>
+        <v>4407.53</v>
+      </c>
+      <c r="C29">
+        <v>1663.76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <f t="shared" si="0"/>
+        <v>4295.95</v>
+      </c>
+      <c r="C30">
+        <v>1775.34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <f t="shared" si="0"/>
+        <v>4267.29</v>
+      </c>
+      <c r="C31">
+        <v>1804</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <f t="shared" si="0"/>
+        <v>4236.33</v>
+      </c>
+      <c r="C32">
+        <v>1834.96</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <f t="shared" si="0"/>
+        <v>4235.21</v>
+      </c>
+      <c r="C33">
+        <v>1836.08</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <f t="shared" si="0"/>
+        <v>4192.04</v>
+      </c>
+      <c r="C34">
+        <v>1879.25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <f t="shared" si="0"/>
+        <v>4170.2</v>
+      </c>
+      <c r="C35">
+        <v>1901.09</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <f t="shared" si="0"/>
+        <v>4119.5</v>
+      </c>
+      <c r="C36">
+        <v>1951.79</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <f t="shared" si="0"/>
+        <v>4008.0099999999998</v>
+      </c>
+      <c r="C37">
+        <v>2063.2800000000002</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <f t="shared" si="0"/>
+        <v>3983.29</v>
+      </c>
+      <c r="C38">
+        <v>2088</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <f t="shared" si="0"/>
+        <v>3952.48</v>
+      </c>
+      <c r="C39">
+        <v>2118.81</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <f t="shared" si="0"/>
+        <v>3893.17</v>
+      </c>
+      <c r="C40">
+        <v>2178.12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <f t="shared" si="0"/>
+        <v>3876.07</v>
+      </c>
+      <c r="C41">
+        <v>2195.2199999999998</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <f t="shared" si="0"/>
+        <v>3811.29</v>
+      </c>
+      <c r="C42">
+        <v>2260</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <f t="shared" si="0"/>
+        <v>3766.29</v>
+      </c>
+      <c r="C43">
+        <v>2305</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <f t="shared" si="0"/>
+        <v>3702.91</v>
+      </c>
+      <c r="C44">
+        <v>2368.38</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
+        <f t="shared" si="0"/>
+        <v>3629.29</v>
+      </c>
+      <c r="C45">
+        <v>2442</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
+        <f t="shared" si="0"/>
+        <v>3592.29</v>
+      </c>
+      <c r="C46">
+        <v>2479</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
+        <f t="shared" si="0"/>
+        <v>3564.47</v>
+      </c>
+      <c r="C47">
+        <v>2506.8200000000002</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <f t="shared" si="0"/>
+        <v>3515.29</v>
+      </c>
+      <c r="C48">
+        <v>2556</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <f t="shared" si="0"/>
+        <v>3288.29</v>
+      </c>
+      <c r="C49">
+        <v>2783</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
+        <f t="shared" si="0"/>
+        <v>3256.98</v>
+      </c>
+      <c r="C50">
+        <v>2814.31</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <f t="shared" si="0"/>
+        <v>3198.29</v>
+      </c>
+      <c r="C51">
+        <v>2873</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <f t="shared" si="0"/>
+        <v>3142.29</v>
+      </c>
+      <c r="C52">
+        <v>2929</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
+        <f t="shared" si="0"/>
+        <v>3111.29</v>
+      </c>
+      <c r="C53">
+        <v>2960</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
+        <f t="shared" si="0"/>
+        <v>3073.29</v>
+      </c>
+      <c r="C54">
+        <v>2998</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
+        <f t="shared" si="0"/>
+        <v>2981.29</v>
+      </c>
+      <c r="C55">
+        <v>3090</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
+        <f t="shared" si="0"/>
+        <v>2936.29</v>
+      </c>
+      <c r="C56">
+        <v>3135</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
+        <f t="shared" si="0"/>
+        <v>2924.29</v>
+      </c>
+      <c r="C57">
+        <v>3147</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="1">
+        <f t="shared" si="0"/>
+        <v>2829.29</v>
+      </c>
+      <c r="C58">
+        <v>3242</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="1">
+        <f t="shared" si="0"/>
+        <v>2814.29</v>
+      </c>
+      <c r="C59">
+        <v>3257</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="1">
+        <f t="shared" si="0"/>
+        <v>2784.09</v>
+      </c>
+      <c r="C60">
+        <v>3287.2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="1">
+        <f t="shared" si="0"/>
+        <v>2707.29</v>
+      </c>
+      <c r="C61">
+        <v>3364</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="1">
+        <f t="shared" si="0"/>
+        <v>2683.29</v>
+      </c>
+      <c r="C62">
+        <v>3388</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="1">
+        <f t="shared" si="0"/>
+        <v>2628.29</v>
+      </c>
+      <c r="C63">
+        <v>3443</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" s="1">
+        <f t="shared" si="0"/>
+        <v>2575.29</v>
+      </c>
+      <c r="C64">
+        <v>3496</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" s="1">
+        <f t="shared" si="0"/>
+        <v>2524.29</v>
+      </c>
+      <c r="C65">
+        <v>3547</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.1499999999996362</v>
+      </c>
+      <c r="C66">
+        <v>6071.44</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.53999999999996362</v>
+      </c>
+      <c r="C67">
+        <v>6071.83</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" s="1">
+        <f t="shared" ref="A68:A75" si="1">$E$1-C68</f>
+        <v>-4.819999999999709</v>
+      </c>
+      <c r="C68">
+        <v>6076.11</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" s="1">
+        <f t="shared" si="1"/>
+        <v>-6.1000000000003638</v>
+      </c>
+      <c r="C69">
+        <v>6077.39</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" s="1">
+        <f t="shared" si="1"/>
+        <v>-13.989999999999782</v>
+      </c>
+      <c r="C70">
+        <v>6085.28</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" s="1">
+        <f t="shared" si="1"/>
+        <v>-14.930000000000291</v>
+      </c>
+      <c r="C71">
+        <v>6086.22</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" s="1">
+        <f t="shared" si="1"/>
+        <v>-20.789999999999964</v>
+      </c>
+      <c r="C72">
+        <v>6092.08</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" s="1">
+        <f t="shared" si="1"/>
+        <v>-22.409999999999854</v>
+      </c>
+      <c r="C73">
+        <v>6093.7</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" s="1">
+        <f t="shared" si="1"/>
+        <v>-29.210000000000036</v>
+      </c>
+      <c r="C74">
+        <v>6100.5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" s="1">
+        <f t="shared" si="1"/>
+        <v>-47.710000000000036</v>
+      </c>
+      <c r="C75">
+        <v>6119</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B76" s="4">
+        <f>SUM(B3:B75)</f>
+        <v>0</v>
+      </c>
+      <c r="C76" s="5">
+        <f>(B76/G1)*100</f>
+        <v>0</v>
+      </c>
+      <c r="D76" s="4" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>